<commit_message>
correct typo mean list
</commit_message>
<xml_diff>
--- a/Work_table_with_lables.xlsx
+++ b/Work_table_with_lables.xlsx
@@ -469,7 +469,7 @@
         <v>20.38999938964844</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -489,7 +489,7 @@
         <v>21.07999992370605</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -509,7 +509,7 @@
         <v>20.67000007629395</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -549,7 +549,7 @@
         <v>20.88999938964844</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -569,7 +569,7 @@
         <v>21.35000038146973</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -629,7 +629,7 @@
         <v>21.5</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -669,7 +669,7 @@
         <v>21.82999992370605</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -689,7 +689,7 @@
         <v>21.1299991607666</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -709,7 +709,7 @@
         <v>22.72999954223633</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -729,7 +729,7 @@
         <v>24.04000091552734</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -749,7 +749,7 @@
         <v>21.06999969482422</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -769,7 +769,7 @@
         <v>22.89999961853027</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -909,7 +909,7 @@
         <v>21.03000068664551</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -949,7 +949,7 @@
         <v>20.8700008392334</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -989,7 +989,7 @@
         <v>22.54999923706055</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1029,7 +1029,7 @@
         <v>22.51000022888184</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1049,7 +1049,7 @@
         <v>23.01000022888184</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1069,7 +1069,7 @@
         <v>21.34000015258789</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1089,7 +1089,7 @@
         <v>22.52000045776367</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1129,7 +1129,7 @@
         <v>20.36000061035156</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1149,7 +1149,7 @@
         <v>21.96999931335449</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1169,7 +1169,7 @@
         <v>19.52000045776367</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1189,7 +1189,7 @@
         <v>20.57999992370605</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1209,7 +1209,7 @@
         <v>20.79000091552734</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1229,7 +1229,7 @@
         <v>20.93000030517578</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1249,7 +1249,7 @@
         <v>20.57999992370605</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1269,7 +1269,7 @@
         <v>21.3799991607666</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1289,7 +1289,7 @@
         <v>21.90999984741211</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1309,7 +1309,7 @@
         <v>22.11000061035156</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1329,7 +1329,7 @@
         <v>21.89999961853027</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1369,7 +1369,7 @@
         <v>21.42000007629395</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -1409,7 +1409,7 @@
         <v>22.36000061035156</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1469,7 +1469,7 @@
         <v>23.90999984741211</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1529,7 +1529,7 @@
         <v>21.30999946594238</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1569,7 +1569,7 @@
         <v>22.04000091552734</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1589,7 +1589,7 @@
         <v>20.6200008392334</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1609,7 +1609,7 @@
         <v>21.48999977111816</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1629,7 +1629,7 @@
         <v>20.78000068664551</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1649,7 +1649,7 @@
         <v>22.29000091552734</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1669,7 +1669,7 @@
         <v>20.95999908447266</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -1689,7 +1689,7 @@
         <v>21.92000007629395</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1709,7 +1709,7 @@
         <v>21.93000030517578</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1729,7 +1729,7 @@
         <v>21.20999908447266</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1789,7 +1789,7 @@
         <v>21.29000091552734</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1829,7 +1829,7 @@
         <v>22.13999938964844</v>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1849,7 +1849,7 @@
         <v>22.1299991607666</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1869,7 +1869,7 @@
         <v>21.69000053405762</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1889,7 +1889,7 @@
         <v>20.8700008392334</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1909,7 +1909,7 @@
         <v>21.90999984741211</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1929,7 +1929,7 @@
         <v>21.8799991607666</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1949,7 +1949,7 @@
         <v>22.48999977111816</v>
       </c>
       <c r="F76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1969,7 +1969,7 @@
         <v>22.38999938964844</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1989,7 +1989,7 @@
         <v>21.1299991607666</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2009,7 +2009,7 @@
         <v>21.97999954223633</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -2029,7 +2029,7 @@
         <v>22.54999923706055</v>
       </c>
       <c r="F80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2049,7 +2049,7 @@
         <v>24.77000045776367</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2109,7 +2109,7 @@
         <v>20.95999908447266</v>
       </c>
       <c r="F84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2149,7 +2149,7 @@
         <v>21.34000015258789</v>
       </c>
       <c r="F86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2169,7 +2169,7 @@
         <v>21.19000053405762</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -2189,7 +2189,7 @@
         <v>21.8700008392334</v>
       </c>
       <c r="F88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2209,7 +2209,7 @@
         <v>21.20999908447266</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -2269,7 +2269,7 @@
         <v>22.52000045776367</v>
       </c>
       <c r="F92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2329,7 +2329,7 @@
         <v>20.22999954223633</v>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -2369,7 +2369,7 @@
         <v>21.68000030517578</v>
       </c>
       <c r="F97" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2449,7 +2449,7 @@
         <v>21.28000068664551</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -2489,7 +2489,7 @@
         <v>21.20000076293945</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -2509,7 +2509,7 @@
         <v>21.94000053405762</v>
       </c>
       <c r="F104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -2549,7 +2549,7 @@
         <v>19.82999992370605</v>
       </c>
       <c r="F106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -2589,7 +2589,7 @@
         <v>22.54999923706055</v>
       </c>
       <c r="F108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2609,7 +2609,7 @@
         <v>21.47999954223633</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -2629,7 +2629,7 @@
         <v>21.06999969482422</v>
       </c>
       <c r="F110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -2669,7 +2669,7 @@
         <v>20.47999954223633</v>
       </c>
       <c r="F112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -2689,7 +2689,7 @@
         <v>22.90999984741211</v>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
@@ -2789,7 +2789,7 @@
         <v>20.35000038146973</v>
       </c>
       <c r="F118" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
@@ -2809,7 +2809,7 @@
         <v>20.75</v>
       </c>
       <c r="F119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -2829,7 +2829,7 @@
         <v>20.93000030517578</v>
       </c>
       <c r="F120" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
@@ -2869,7 +2869,7 @@
         <v>22.63999938964844</v>
       </c>
       <c r="F122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -2909,7 +2909,7 @@
         <v>22.3799991607666</v>
       </c>
       <c r="F124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -3029,7 +3029,7 @@
         <v>20.29000091552734</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -3049,7 +3049,7 @@
         <v>21.52000045776367</v>
       </c>
       <c r="F131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -3069,7 +3069,7 @@
         <v>21.70999908447266</v>
       </c>
       <c r="F132" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -3089,7 +3089,7 @@
         <v>20.51000022888184</v>
       </c>
       <c r="F133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -3149,7 +3149,7 @@
         <v>21.14999961853027</v>
       </c>
       <c r="F136" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -3169,7 +3169,7 @@
         <v>20.59000015258789</v>
       </c>
       <c r="F137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -3189,7 +3189,7 @@
         <v>21.46999931335449</v>
       </c>
       <c r="F138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -3209,7 +3209,7 @@
         <v>22.07999992370605</v>
       </c>
       <c r="F139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -3229,7 +3229,7 @@
         <v>21.60000038146973</v>
       </c>
       <c r="F140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -3249,7 +3249,7 @@
         <v>21.92000007629395</v>
       </c>
       <c r="F141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -3269,7 +3269,7 @@
         <v>21.90999984741211</v>
       </c>
       <c r="F142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -3289,7 +3289,7 @@
         <v>21.78000068664551</v>
       </c>
       <c r="F143" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -3309,7 +3309,7 @@
         <v>21.21999931335449</v>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>